<commit_message>
Checking in MEDEMD.XLSX file
</commit_message>
<xml_diff>
--- a/utilities/Excel_Sheets/Products/MEDEMD.xlsx
+++ b/utilities/Excel_Sheets/Products/MEDEMD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10575" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10575" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Cases" sheetId="5" r:id="rId1"/>
@@ -693,10 +693,10 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -758,7 +758,7 @@
       </c>
       <c r="C2" s="19">
         <f ca="1">TODAY()</f>
-        <v>43262</v>
+        <v>43266</v>
       </c>
       <c r="D2" s="8">
         <v>3</v>
@@ -795,7 +795,7 @@
       </c>
       <c r="C4" s="18">
         <f ca="1">TODAY()</f>
-        <v>43262</v>
+        <v>43266</v>
       </c>
       <c r="D4" s="11">
         <v>2</v>
@@ -832,7 +832,7 @@
       </c>
       <c r="C6" s="17">
         <f ca="1">TODAY()</f>
-        <v>43262</v>
+        <v>43266</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
@@ -1190,10 +1190,10 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:L163"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1259,7 +1259,7 @@
       </c>
       <c r="C2" s="17">
         <f ca="1">TODAY()</f>
-        <v>43262</v>
+        <v>43266</v>
       </c>
       <c r="D2" s="5">
         <v>1</v>
@@ -6614,10 +6614,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M9"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>